<commit_message>
Small fixes to questions
</commit_message>
<xml_diff>
--- a/matlab_attempt/Excel problems/Data questions.xlsx
+++ b/matlab_attempt/Excel problems/Data questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\QMB-Problem-Maker\matlab_attempt\Excel problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D46DC86-9ECE-40D7-B729-78F00F832B27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD1DBDF-72C7-4B52-B971-486FB4C917D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="11" xr2:uid="{BC6FDD6A-A67B-40E6-83ED-ED8A835A9503}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="9" xr2:uid="{BC6FDD6A-A67B-40E6-83ED-ED8A835A9503}"/>
   </bookViews>
   <sheets>
     <sheet name="CG5.1.3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,8 @@
     <sheet name="CG5.3.1" sheetId="12" r:id="rId10"/>
     <sheet name="CG5.3.2" sheetId="13" r:id="rId11"/>
     <sheet name="CG5.3.3" sheetId="14" r:id="rId12"/>
-    <sheet name="Unused" sheetId="7" r:id="rId13"/>
+    <sheet name="CG5.3.4" sheetId="15" r:id="rId13"/>
+    <sheet name="Unused" sheetId="7" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4993" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5213" uniqueCount="899">
   <si>
     <t>questionText</t>
   </si>
@@ -3930,6 +3931,76 @@
   </si>
   <si>
     <t>D22</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The line $im = imread('FILESTR')/$ caused an error because Matlab could not find "FILESTR". Matlab will first search in the current directory, followed by each folder on the patch. Therefore, there are multiple ways to possibly fix this error.&lt;/p&gt;
+&lt;br/&gt;
+&lt;p&gt;The possible answers here are:
+&lt;ul&gt;EXPLAIN&lt;/ul&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;There are several ways you could load this image.&lt;/p&gt;
+&lt;br/&gt;
+&lt;p&gt;The possible answers here are:
+&lt;ul&gt;EXPLAIN&lt;/ul&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>path1_review</t>
+  </si>
+  <si>
+    <t>path2_review</t>
+  </si>
+  <si>
+    <t>path3_review</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You have an file named "FILESTR" located in the folder "PATHSTR". You type $myTable = readtable('FILESTR')/$ into the command line and receive an error message saying that "FILESTR" does not exist. You double-check your spelling and find no mistakes. You also check and confirm that the file does exist in "PATHSTR". &lt;/p&gt;&lt;p&gt;What are some ways you could fix this error?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>[answers, correctness, pathstr, filestr, explanation] = path1_review();</t>
+  </si>
+  <si>
+    <t>[answers, correctness, pathstr, filestr, explanation] = path2_review();</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You have a data file named "FILESTR" located in the folder "PATHSTR".  Which choice(s) below would successfully load this file into Matlab?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>[answers, correctness, pathstr, filestr, explanation] = path3_review();</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You have a data file named "FILESTR" located in the folder "PATHSTR". Your current directory is a different folder. Which choice(s) below would successfully load this file into a variable named $myTable/$?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Download &lt;a href="/static/random_table_ID.csv" target="_blank"&gt;this file&lt;/a&gt; and load it into Matlab by dragging the file from your desktop into the Command Window. If you are using Matlab Online, you will need to upload the file first. 
+&lt;/p&gt;
+&lt;p&gt;
+A user interface will open that will allow you to import the data as a table. You can finish the import process by clicking "Import Selection" near the top-right of the window.
+&lt;/p&gt;
+&lt;p&gt;
+How many observations does this data have?
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>data51.4</t>
+  </si>
+  <si>
+    <t>FILEID</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Download &lt;a href="/static/random_table_FILEID.csv" target="_blank"&gt;this file&lt;/a&gt; and load it into Matlab by dragging the file from your desktop into the Command Window. If you are using Matlab Online, you will need to upload the file first. 
+&lt;/p&gt;
+&lt;p&gt;
+A user interface will open that will allow you to import the data as a table. You can finish the import process by clicking "Import Selection" near the top-right of the window.
+&lt;/p&gt;
+&lt;p&gt;
+What is the ORD1 observation of the $VAR_NAME/$ variable?
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>T = readtable('Data\random_table_FILEID.csv');</t>
   </si>
 </sst>
 </file>
@@ -3985,7 +4056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4041,6 +4112,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4357,8 +4430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABA62E7-B975-412E-89FE-9864931B8B79}">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5477,8 +5550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5B8C05-919E-4A16-AAB9-DDFCD7F7F9FF}">
   <dimension ref="A1:E217"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="C180" sqref="C180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7271,13 +7344,13 @@
     </row>
     <row r="166" spans="1:5" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>862</v>
+        <v>875</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>865</v>
+        <v>894</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -7398,13 +7471,13 @@
     </row>
     <row r="178" spans="1:4" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>866</v>
+        <v>897</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -7412,7 +7485,7 @@
         <v>1</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>5</v>
+        <v>896</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>492</v>
@@ -7426,7 +7499,7 @@
         <v>2</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>863</v>
+        <v>898</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -7613,7 +7686,7 @@
     </row>
     <row r="198" spans="1:5" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>878</v>
+        <v>895</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>0</v>
@@ -9622,8 +9695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5617C5FD-31B0-40B2-B234-37C58CD07772}">
   <dimension ref="A1:XFD150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19435,6 +19508,980 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4563B77E-3990-4C7B-A385-8D3DA8FF1988}">
+  <dimension ref="A1:F72"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="83.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>883</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="30"/>
+    </row>
+    <row r="27" spans="1:6" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>816</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
+      <c r="B48" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+    </row>
+    <row r="49" spans="1:6" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="13"/>
+      <c r="B49" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="30"/>
+    </row>
+    <row r="50" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="B62" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="B67" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+      <c r="B68" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="B69" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+      <c r="B70" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>884</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="13"/>
+      <c r="B72" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C61819-6B96-4D9A-9FFA-545F814BD4B1}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -19598,8 +20645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46410BC6-4A56-41D6-B9E7-CD9E9C5E16DF}">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>